<commit_message>
Terminación de parámetros de procesos y socialización enm reunión del 10 de abril
</commit_message>
<xml_diff>
--- a/01 Documentación/01 Investigación fabricación de bicicletas/03 Código y análisis/Valores e información asociada al proceso.xlsx
+++ b/01 Documentación/01 Investigación fabricación de bicicletas/03 Código y análisis/Valores e información asociada al proceso.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo7s\Documents\Universidad\03 APM\04 Gitrespository\Proyecto_APM\01 Documentación\01 Investigación fabricación de bicicletas\03 Código y análisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E145A46-F584-4715-B18D-EA4D97021929}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE154AF2-6D2B-4FE0-BF07-0CD60496610E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiempos Produccion" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="128">
   <si>
     <t>Numero
  de 
@@ -399,7 +399,52 @@
     <t>und x semana</t>
   </si>
   <si>
-    <t>estaciones</t>
+    <t>linea</t>
+  </si>
+  <si>
+    <t>Umax</t>
+  </si>
+  <si>
+    <t>Utilización máxima</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Utilización</t>
+  </si>
+  <si>
+    <t>Umin</t>
+  </si>
+  <si>
+    <t>Utilización mínima</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Tno</t>
+  </si>
+  <si>
+    <t>Tiempos no operativos</t>
+  </si>
+  <si>
+    <t>MLTmax</t>
+  </si>
+  <si>
+    <t>MLT</t>
+  </si>
+  <si>
+    <t>MLTmin</t>
+  </si>
+  <si>
+    <t>Manufacturing Lead Time Max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturing Lead Time </t>
+  </si>
+  <si>
+    <t>Manufacturing Lead Time Min</t>
   </si>
 </sst>
 </file>
@@ -408,7 +453,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -503,7 +548,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -542,7 +587,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -560,16 +605,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -591,6 +633,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -890,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:N34"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1729,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890FC51D-AFFD-469A-9879-815ABD787FD2}">
   <dimension ref="B3:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:G44"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1758,14 +1806,14 @@
       <c r="E3" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="J3" s="29" t="s">
+      <c r="G3" s="31"/>
+      <c r="J3" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="K3" s="29" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -1773,7 +1821,7 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1786,7 +1834,7 @@
       <c r="E4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="20">
         <v>4.2173611111111109</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -1804,7 +1852,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>60</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1816,7 +1864,7 @@
       <c r="E5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="21">
         <v>0.33333333333333331</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -1834,7 +1882,7 @@
       </c>
     </row>
     <row r="6" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>61</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1860,13 +1908,13 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="22">
         <f>D5/D6</f>
         <v>5.9259259259259256</v>
       </c>
@@ -1887,7 +1935,7 @@
       </c>
     </row>
     <row r="8" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1913,13 +1961,13 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>62</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="23">
         <v>0.15</v>
       </c>
       <c r="E9" s="2"/>
@@ -1937,7 +1985,7 @@
       </c>
     </row>
     <row r="10" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>63</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1964,7 +2012,7 @@
       </c>
     </row>
     <row r="11" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1991,13 +2039,13 @@
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="26" t="s">
         <v>65</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="22">
         <f>D5/D10</f>
         <v>5.1529790660225441</v>
       </c>
@@ -2018,13 +2066,13 @@
       </c>
     </row>
     <row r="13" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>77</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <f>D5/D6</f>
         <v>5.9259259259259256</v>
       </c>
@@ -2045,13 +2093,13 @@
       </c>
     </row>
     <row r="14" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="26" t="s">
         <v>66</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="22">
         <f>D5/D11</f>
         <v>6.9716775599128544</v>
       </c>
@@ -2072,7 +2120,7 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="26" t="s">
         <v>67</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -2098,7 +2146,7 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="26" t="s">
         <v>74</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -2124,13 +2172,13 @@
       </c>
     </row>
     <row r="17" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="26" t="s">
         <v>79</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="27">
         <f>D16+D15*D12</f>
         <v>417.39130434782606</v>
       </c>
@@ -2151,7 +2199,7 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="26" t="s">
         <v>75</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -2178,7 +2226,7 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>80</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -2205,13 +2253,13 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="26" t="s">
         <v>85</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="22">
         <f>D17/D15</f>
         <v>5.1529790660225441</v>
       </c>
@@ -2232,13 +2280,13 @@
       </c>
     </row>
     <row r="21" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="26" t="s">
         <v>83</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="22">
         <f>D18/D15</f>
         <v>5.9259259259259256</v>
       </c>
@@ -2259,13 +2307,13 @@
       </c>
     </row>
     <row r="22" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="26" t="s">
         <v>86</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="22">
         <f>D19/D15</f>
         <v>6.9716775599128544</v>
       </c>
@@ -2286,13 +2334,13 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="26" t="s">
         <v>94</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="22">
         <f>60/D20</f>
         <v>11.643750000000001</v>
       </c>
@@ -2313,13 +2361,13 @@
       </c>
     </row>
     <row r="24" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="26" t="s">
         <v>91</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="22">
         <f>60/D21</f>
         <v>10.125</v>
       </c>
@@ -2330,13 +2378,13 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="26" t="s">
         <v>95</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="22">
         <f>60/D22</f>
         <v>8.6062499999999993</v>
       </c>
@@ -2347,7 +2395,7 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="26" t="s">
         <v>98</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -2363,7 +2411,7 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>100</v>
       </c>
       <c r="C27" s="16" t="s">
@@ -2379,7 +2427,7 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="17" t="s">
@@ -2393,6 +2441,16 @@
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
+      <c r="J28" s="1">
+        <v>2019</v>
+      </c>
+      <c r="K28" s="1">
+        <v>18267</v>
+      </c>
+      <c r="L28">
+        <f>K28/365</f>
+        <v>50.046575342465751</v>
+      </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="17" t="s">
@@ -2410,6 +2468,16 @@
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
+      <c r="J29" s="1">
+        <v>2020</v>
+      </c>
+      <c r="K29" s="1">
+        <v>18601</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ref="L29:L32" si="1">K29/365</f>
+        <v>50.961643835616435</v>
+      </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="17" t="s">
@@ -2427,6 +2495,16 @@
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
+      <c r="J30" s="1">
+        <v>2021</v>
+      </c>
+      <c r="K30" s="1">
+        <v>18887</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>51.745205479452054</v>
+      </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="17" t="s">
@@ -2444,120 +2522,256 @@
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
+      <c r="J31" s="1">
+        <v>2022</v>
+      </c>
+      <c r="K31" s="1">
+        <v>19204</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>52.613698630136987</v>
+      </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="17"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="B32" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="2">
+        <f>(D29/D30)*100</f>
+        <v>114.99999999999999</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="J32" s="1">
+        <v>2023</v>
+      </c>
+      <c r="K32" s="1">
+        <v>19504</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="1"/>
+        <v>53.435616438356163</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B33" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" s="2">
+        <f>(D30/D30)*100</f>
+        <v>100</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="17"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B34" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" s="2">
+        <f>(D31/D30)*100</f>
+        <v>85</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B35" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="J35" s="1">
+        <v>2019</v>
+      </c>
+      <c r="K35" s="1">
+        <f>365*L35</f>
+        <v>29565</v>
+      </c>
+      <c r="L35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B36" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="8">
+        <f>D26*(D16+D15*D12+D35)</f>
+        <v>417.39130434782606</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="J36" s="1">
+        <v>2020</v>
+      </c>
+      <c r="K36" s="1">
+        <f t="shared" ref="K36:K39" si="2">365*L36</f>
+        <v>29565</v>
+      </c>
+      <c r="L36">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B37" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="8">
+        <f>D26*(D16+D15*D13+D35)</f>
+        <v>480</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="J37" s="1">
+        <v>2021</v>
+      </c>
+      <c r="K37" s="1">
+        <f t="shared" si="2"/>
+        <v>29565</v>
+      </c>
+      <c r="L37">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B38" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="8">
+        <f>D26*(D16+D15*D14+D35)</f>
+        <v>564.70588235294122</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="J38" s="1">
+        <v>2022</v>
+      </c>
+      <c r="K38" s="1">
+        <f t="shared" si="2"/>
+        <v>29565</v>
+      </c>
+      <c r="L38">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="5"/>
+      <c r="J39" s="1">
+        <v>2023</v>
+      </c>
+      <c r="K39" s="1">
+        <f t="shared" si="2"/>
+        <v>29565</v>
+      </c>
+      <c r="L39">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
     </row>

</xml_diff>

<commit_message>
Se finaliza el DF del proceso manual.
Se realiza el diagrama de flujo del proceso manual, estación por estación, teniendo en cuenta los tiempos de proceso y las cantidades de operaciones a realizar.
</commit_message>
<xml_diff>
--- a/01 Documentación/01 Investigación fabricación de bicicletas/03 Código y análisis/Valores e información asociada al proceso.xlsx
+++ b/01 Documentación/01 Investigación fabricación de bicicletas/03 Código y análisis/Valores e información asociada al proceso.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo7s\Documents\Universidad\03 APM\04 Gitrespository\Proyecto_APM\01 Documentación\01 Investigación fabricación de bicicletas\03 Código y análisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE154AF2-6D2B-4FE0-BF07-0CD60496610E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2B5E71-5D44-4043-97D3-7E4134D50E4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiempos Produccion" sheetId="1" r:id="rId1"/>
     <sheet name="Prmtrs Produc Manual" sheetId="2" r:id="rId2"/>
+    <sheet name="Demanda" sheetId="3" r:id="rId3"/>
+    <sheet name="Materia prima" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="178">
   <si>
     <t>Numero
  de 
@@ -445,6 +447,165 @@
   </si>
   <si>
     <t>Manufacturing Lead Time Min</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Dias habiles</t>
+  </si>
+  <si>
+    <t>Producción Diaría
+Necesaría</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Junio</t>
+  </si>
+  <si>
+    <t>Julio</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Septiembre</t>
+  </si>
+  <si>
+    <t>Octubre</t>
+  </si>
+  <si>
+    <t>Noviembre</t>
+  </si>
+  <si>
+    <t>Diciembre</t>
+  </si>
+  <si>
+    <t>Producción 
+necesaria [%]</t>
+  </si>
+  <si>
+    <t>Producción
+necesaria [und]</t>
+  </si>
+  <si>
+    <t>Tubos</t>
+  </si>
+  <si>
+    <t>Platina soporte llanta</t>
+  </si>
+  <si>
+    <t>Platina soporte CC</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>DESCRIPCION</t>
+  </si>
+  <si>
+    <t>Platina contra freno</t>
+  </si>
+  <si>
+    <t>Platina reflector</t>
+  </si>
+  <si>
+    <t>Collarín tubo sillín</t>
+  </si>
+  <si>
+    <t>Lamina cubre cadenas</t>
+  </si>
+  <si>
+    <t>Cubetas</t>
+  </si>
+  <si>
+    <t>Juego caja central</t>
+  </si>
+  <si>
+    <t>Plato</t>
+  </si>
+  <si>
+    <t>Biela tipo Z</t>
+  </si>
+  <si>
+    <t>Tornillos 3/16x3/8</t>
+  </si>
+  <si>
+    <t>Sillín</t>
+  </si>
+  <si>
+    <t>Tubo sillín</t>
+  </si>
+  <si>
+    <t>Tornillo 1/4"x2" con tuerca</t>
+  </si>
+  <si>
+    <t>Juego de dirección</t>
+  </si>
+  <si>
+    <t>Caña de Dirección</t>
+  </si>
+  <si>
+    <t>Manubrio</t>
+  </si>
+  <si>
+    <t>Mangos</t>
+  </si>
+  <si>
+    <t>rin #26</t>
+  </si>
+  <si>
+    <t>Manzana con freno</t>
+  </si>
+  <si>
+    <t>Juego de rayos con cabezilla</t>
+  </si>
+  <si>
+    <t>Mazana delantera</t>
+  </si>
+  <si>
+    <t>Cinta de protección para Neumático</t>
+  </si>
+  <si>
+    <t>Juego de piñon</t>
+  </si>
+  <si>
+    <t>cadena</t>
+  </si>
+  <si>
+    <t>Juego de Stickers</t>
+  </si>
+  <si>
+    <t>CANTIDAD 
+POR 
+PROCESO</t>
+  </si>
+  <si>
+    <t>CANTIDAD 
+POR 
+BICICLETA</t>
+  </si>
+  <si>
+    <t>Ventas 
+proyectadas 
+por año</t>
   </si>
 </sst>
 </file>
@@ -455,7 +616,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,6 +650,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -548,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -641,6 +808,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,15 +1112,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:N34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
     <col min="3" max="3" width="37.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="19.21875" bestFit="1" customWidth="1"/>
@@ -1052,39 +1226,39 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
+    <row r="6" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="17">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="17">
         <v>111.7</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="17">
         <v>486</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="32">
         <f>(D6/E6)*60</f>
         <v>13.790123456790123</v>
       </c>
-      <c r="G6" s="2" t="str">
+      <c r="G6" s="17" t="str">
         <f t="shared" si="0"/>
         <v>1:51,7</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="32">
         <f t="shared" si="1"/>
         <v>23.270833333333336</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
@@ -1131,11 +1305,11 @@
         <v>875.8</v>
       </c>
       <c r="E8" s="7">
-        <v>972</v>
+        <v>2025</v>
       </c>
       <c r="F8" s="8">
         <f t="shared" si="2"/>
-        <v>54.061728395061728</v>
+        <v>25.949629629629626</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1154,39 +1328,39 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
+    <row r="9" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="17">
         <v>6</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="17">
         <v>22.8</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="17">
         <v>81</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="32">
         <f t="shared" si="2"/>
         <v>16.888888888888889</v>
       </c>
-      <c r="G9" s="2" t="str">
+      <c r="G9" s="17" t="str">
         <f t="shared" si="0"/>
         <v>0:22,8</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="32">
         <f t="shared" si="1"/>
         <v>4.75</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -1392,243 +1566,243 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="2">
+    <row r="16" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="17">
         <v>15</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="17">
         <v>397.5</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="17">
         <v>81</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="32">
         <f t="shared" si="2"/>
         <v>294.44444444444446</v>
       </c>
-      <c r="G16" s="2" t="str">
+      <c r="G16" s="17" t="str">
         <f t="shared" si="0"/>
         <v>6:37,5</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="32">
         <f t="shared" si="1"/>
         <v>82.8125</v>
       </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="2">
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+    </row>
+    <row r="17" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="17">
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="17">
         <v>399.1</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="17">
         <v>81</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="32">
         <f t="shared" si="2"/>
         <v>295.62962962962968</v>
       </c>
-      <c r="G17" s="2" t="str">
+      <c r="G17" s="17" t="str">
         <f t="shared" si="0"/>
         <v>6:39,1</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="32">
         <f t="shared" si="1"/>
         <v>83.145833333333343</v>
       </c>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+    </row>
+    <row r="18" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="17">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="17">
         <v>335.2</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="17">
         <v>162</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="32">
         <f t="shared" si="2"/>
         <v>124.14814814814815</v>
       </c>
-      <c r="G18" s="2" t="str">
+      <c r="G18" s="17" t="str">
         <f t="shared" si="0"/>
         <v>5:35,2</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="32">
         <f t="shared" si="1"/>
         <v>69.833333333333343</v>
       </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="2">
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+    </row>
+    <row r="19" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="17">
         <v>18</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="17">
         <v>223.4</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="17">
         <v>162</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="32">
         <f t="shared" si="2"/>
         <v>82.740740740740748</v>
       </c>
-      <c r="G19" s="2" t="str">
+      <c r="G19" s="17" t="str">
         <f t="shared" si="0"/>
         <v>3:43,4</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="32">
         <f t="shared" si="1"/>
         <v>46.541666666666671</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="2">
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+    </row>
+    <row r="20" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="17">
         <v>19</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="17">
         <v>388.2</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="17">
         <v>162</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="32">
         <f t="shared" si="2"/>
         <v>143.77777777777777</v>
       </c>
-      <c r="G20" s="2" t="str">
+      <c r="G20" s="17" t="str">
         <f t="shared" si="0"/>
         <v>6:28,2</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="32">
         <f t="shared" si="1"/>
         <v>80.875</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="2">
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+    </row>
+    <row r="21" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="17">
         <v>20</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="17">
         <v>324.8</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="17">
         <v>81</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="32">
         <f t="shared" si="2"/>
         <v>240.59259259259258</v>
       </c>
-      <c r="G21" s="2" t="str">
+      <c r="G21" s="17" t="str">
         <f t="shared" si="0"/>
         <v>5:24,8</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="32">
         <f t="shared" si="1"/>
         <v>67.666666666666657</v>
       </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="2">
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+    </row>
+    <row r="22" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="17">
         <v>21</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="17">
         <v>96.5</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="17">
         <v>81</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="32">
         <f t="shared" si="2"/>
         <v>71.481481481481481</v>
       </c>
-      <c r="G22" s="2" t="str">
+      <c r="G22" s="17" t="str">
         <f t="shared" si="0"/>
         <v>1:36,5</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="8">
+      <c r="I22" s="32">
         <f t="shared" si="1"/>
         <v>20.104166666666668</v>
       </c>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="2">
@@ -1777,8 +1951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890FC51D-AFFD-469A-9879-815ABD787FD2}">
   <dimension ref="B3:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2782,4 +2956,685 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DAC816-1EAB-4B11-BF11-B04A3BDA67B0}">
+  <dimension ref="B2:E29"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.5546875" style="1"/>
+    <col min="3" max="3" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="54" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C3" s="2">
+        <v>20120</v>
+      </c>
+      <c r="D3" s="2">
+        <v>249</v>
+      </c>
+      <c r="E3" s="9">
+        <f t="shared" ref="E3:E7" si="0">C3/D3</f>
+        <v>80.803212851405618</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20437</v>
+      </c>
+      <c r="D4" s="2">
+        <v>249</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="0"/>
+        <v>82.07630522088354</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C5" s="2">
+        <v>20739</v>
+      </c>
+      <c r="D5" s="2">
+        <v>248</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="0"/>
+        <v>83.625</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C6" s="2">
+        <v>21050</v>
+      </c>
+      <c r="D6" s="2">
+        <v>251</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="0"/>
+        <v>83.864541832669318</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C7" s="2">
+        <v>21358</v>
+      </c>
+      <c r="D7" s="2">
+        <v>246</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="0"/>
+        <v>86.82113821138212</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="36" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="23">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9">
+        <f>C18*$E$3</f>
+        <v>80.803212851405618</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" ref="D19:D29" si="1">C19*$E$3</f>
+        <v>72.722891566265062</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" si="1"/>
+        <v>72.722891566265062</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="23">
+        <v>0.85</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" si="1"/>
+        <v>68.682730923694777</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="23">
+        <v>1.05</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="1"/>
+        <v>84.843373493975903</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="23">
+        <v>0.95</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="1"/>
+        <v>76.763052208835333</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="23">
+        <v>0.95</v>
+      </c>
+      <c r="D24" s="9">
+        <f t="shared" si="1"/>
+        <v>76.763052208835333</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="23">
+        <v>1</v>
+      </c>
+      <c r="D25" s="9">
+        <f t="shared" si="1"/>
+        <v>80.803212851405618</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="23">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D26" s="9">
+        <f t="shared" si="1"/>
+        <v>88.883534136546189</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="23">
+        <v>1.3</v>
+      </c>
+      <c r="D27" s="9">
+        <f t="shared" si="1"/>
+        <v>105.0441767068273</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="23">
+        <v>1</v>
+      </c>
+      <c r="D28" s="9">
+        <f t="shared" si="1"/>
+        <v>80.803212851405618</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" s="23">
+        <v>1</v>
+      </c>
+      <c r="D29" s="9">
+        <f t="shared" si="1"/>
+        <v>80.803212851405618</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B327D1-8ECB-4B5A-8204-7C39AC8E79CD}">
+  <dimension ref="A3:D30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" ht="54" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="2">
+        <v>84</v>
+      </c>
+      <c r="D4" s="22">
+        <f>C4/81</f>
+        <v>1.037037037037037</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="2">
+        <v>162</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="2">
+        <v>243</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="2">
+        <v>81</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="2">
+        <v>81</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="2">
+        <v>81</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="2">
+        <v>81</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="2">
+        <v>162</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="2">
+        <v>81</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="2">
+        <v>81</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" s="2">
+        <v>81</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="2">
+        <v>243</v>
+      </c>
+      <c r="D15" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" s="2">
+        <v>81</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C17" s="2">
+        <v>81</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="2">
+        <v>81</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" s="2">
+        <v>81</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="2">
+        <v>81</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" s="2">
+        <v>81</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C22" s="2">
+        <v>162</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>20</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C23" s="2">
+        <v>162</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>21</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C24" s="2">
+        <v>81</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" s="2">
+        <v>81</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C26" s="2">
+        <v>162</v>
+      </c>
+      <c r="D26" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>24</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C27" s="2">
+        <v>162</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>26</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" s="2">
+        <v>81</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>27</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" s="2">
+        <v>81</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se avanza en los KPIS y la infraestructura de red utilizada
</commit_message>
<xml_diff>
--- a/01 Documentación/01 Investigación fabricación de bicicletas/03 Código y análisis/Valores e información asociada al proceso.xlsx
+++ b/01 Documentación/01 Investigación fabricación de bicicletas/03 Código y análisis/Valores e información asociada al proceso.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo7s\Documents\Universidad\03 APM\04 Gitrespository\Proyecto_APM\01 Documentación\01 Investigación fabricación de bicicletas\03 Código y análisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2B5E71-5D44-4043-97D3-7E4134D50E4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5ABFC5-7DA4-47DE-AF94-76E419E0A895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiempos Produccion" sheetId="1" r:id="rId1"/>
@@ -805,9 +805,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -815,6 +812,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1112,22 +1112,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:N34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="37.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" ht="75" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1158,7 +1158,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -1192,7 +1192,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -1226,7 +1226,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17">
         <v>3</v>
       </c>
@@ -1239,7 +1239,7 @@
       <c r="E6" s="17">
         <v>486</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="31">
         <f>(D6/E6)*60</f>
         <v>13.790123456790123</v>
       </c>
@@ -1250,17 +1250,17 @@
       <c r="H6" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="31">
         <f t="shared" si="1"/>
         <v>23.270833333333336</v>
       </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -1294,7 +1294,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -1328,7 +1328,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="17">
         <v>6</v>
       </c>
@@ -1341,7 +1341,7 @@
       <c r="E9" s="17">
         <v>81</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="31">
         <f t="shared" si="2"/>
         <v>16.888888888888889</v>
       </c>
@@ -1352,17 +1352,17 @@
       <c r="H9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="31">
         <f t="shared" si="1"/>
         <v>4.75</v>
       </c>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1396,7 +1396,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>9</v>
       </c>
@@ -1430,7 +1430,7 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>11</v>
       </c>
@@ -1464,7 +1464,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="2:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>12</v>
       </c>
@@ -1498,7 +1498,7 @@
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>13</v>
       </c>
@@ -1532,7 +1532,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>14</v>
       </c>
@@ -1566,7 +1566,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="17">
         <v>15</v>
       </c>
@@ -1579,7 +1579,7 @@
       <c r="E16" s="17">
         <v>81</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="31">
         <f t="shared" si="2"/>
         <v>294.44444444444446</v>
       </c>
@@ -1590,17 +1590,17 @@
       <c r="H16" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I16" s="31">
         <f t="shared" si="1"/>
         <v>82.8125</v>
       </c>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-    </row>
-    <row r="17" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+    </row>
+    <row r="17" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
         <v>16</v>
       </c>
@@ -1613,7 +1613,7 @@
       <c r="E17" s="17">
         <v>81</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="31">
         <f t="shared" si="2"/>
         <v>295.62962962962968</v>
       </c>
@@ -1624,17 +1624,17 @@
       <c r="H17" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I17" s="31">
         <f t="shared" si="1"/>
         <v>83.145833333333343</v>
       </c>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-    </row>
-    <row r="18" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+    </row>
+    <row r="18" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="17">
         <v>17</v>
       </c>
@@ -1647,7 +1647,7 @@
       <c r="E18" s="17">
         <v>162</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="31">
         <f t="shared" si="2"/>
         <v>124.14814814814815</v>
       </c>
@@ -1658,17 +1658,17 @@
       <c r="H18" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="32">
+      <c r="I18" s="31">
         <f t="shared" si="1"/>
         <v>69.833333333333343</v>
       </c>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-    </row>
-    <row r="19" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+    </row>
+    <row r="19" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="17">
         <v>18</v>
       </c>
@@ -1681,7 +1681,7 @@
       <c r="E19" s="17">
         <v>162</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="31">
         <f t="shared" si="2"/>
         <v>82.740740740740748</v>
       </c>
@@ -1692,17 +1692,17 @@
       <c r="H19" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="32">
+      <c r="I19" s="31">
         <f t="shared" si="1"/>
         <v>46.541666666666671</v>
       </c>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-    </row>
-    <row r="20" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+    </row>
+    <row r="20" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="17">
         <v>19</v>
       </c>
@@ -1715,7 +1715,7 @@
       <c r="E20" s="17">
         <v>162</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="31">
         <f t="shared" si="2"/>
         <v>143.77777777777777</v>
       </c>
@@ -1726,17 +1726,17 @@
       <c r="H20" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="32">
+      <c r="I20" s="31">
         <f t="shared" si="1"/>
         <v>80.875</v>
       </c>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-    </row>
-    <row r="21" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+    </row>
+    <row r="21" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="17">
         <v>20</v>
       </c>
@@ -1749,7 +1749,7 @@
       <c r="E21" s="17">
         <v>81</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="31">
         <f t="shared" si="2"/>
         <v>240.59259259259258</v>
       </c>
@@ -1760,17 +1760,17 @@
       <c r="H21" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="32">
+      <c r="I21" s="31">
         <f t="shared" si="1"/>
         <v>67.666666666666657</v>
       </c>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-    </row>
-    <row r="22" spans="2:14" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+    </row>
+    <row r="22" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17">
         <v>21</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="E22" s="17">
         <v>81</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="31">
         <f t="shared" si="2"/>
         <v>71.481481481481481</v>
       </c>
@@ -1794,17 +1794,17 @@
       <c r="H22" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="32">
+      <c r="I22" s="31">
         <f t="shared" si="1"/>
         <v>20.104166666666668</v>
       </c>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>22</v>
       </c>
@@ -1838,7 +1838,7 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1853,7 +1853,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -1868,7 +1868,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1876,7 +1876,7 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1884,7 +1884,7 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1892,7 +1892,7 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1900,7 +1900,7 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1908,7 +1908,7 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1916,7 +1916,7 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1924,7 +1924,7 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1932,7 +1932,7 @@
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1951,23 +1951,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890FC51D-AFFD-469A-9879-815ABD787FD2}">
   <dimension ref="B3:L47"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="11.5546875" style="1"/>
-    <col min="10" max="10" width="19.88671875" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="11.5703125" style="1"/>
+    <col min="10" max="10" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>68</v>
       </c>
@@ -1980,10 +1980,10 @@
       <c r="E3" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="31"/>
+      <c r="G3" s="34"/>
       <c r="J3" s="28" t="s">
         <v>89</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
         <v>43</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>4.325925925925926</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
         <v>60</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>4.7506172839506178</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
         <v>61</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>1.3790123456790124</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
         <v>59</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>9.1950617283950606</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
         <v>28</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>10.812345679012346</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
         <v>62</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>0.2814814814814815</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
         <v>63</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>5.9259259259259256</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
         <v>64</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>5.7049382716049388</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
         <v>65</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>0.49876543209876539</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
         <v>77</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>2.2567901234567902</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
         <v>66</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>1.4481481481481482</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
         <v>67</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>1.1012345679012345</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
         <v>74</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>4.9074074074074074</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
         <v>79</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>4.9271604938271611</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
         <v>75</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>4.1382716049382715</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
         <v>80</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>2.7580246913580249</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="26" t="s">
         <v>85</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>4.7925925925925927</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
         <v>83</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>4.0098765432098764</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
         <v>86</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>1.191358024691358</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
         <v>94</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>0.57530864197530862</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
         <v>91</v>
       </c>
@@ -2551,7 +2551,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
         <v>95</v>
       </c>
@@ -2568,7 +2568,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="s">
         <v>98</v>
       </c>
@@ -2584,7 +2584,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="24" t="s">
         <v>100</v>
       </c>
@@ -2600,7 +2600,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
         <v>35</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>50.046575342465751</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
         <v>107</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>50.961643835616435</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
         <v>105</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>51.745205479452054</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
         <v>108</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>52.613698630136987</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
         <v>113</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>53.435616438356163</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
         <v>115</v>
       </c>
@@ -2751,7 +2751,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="17" t="s">
         <v>117</v>
       </c>
@@ -2768,7 +2768,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="17" t="s">
         <v>120</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="17" t="s">
         <v>122</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="17" t="s">
         <v>123</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="17" t="s">
         <v>124</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="5"/>
@@ -2893,7 +2893,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
       <c r="D40" s="5"/>
@@ -2901,7 +2901,7 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
       <c r="D41" s="5"/>
@@ -2909,7 +2909,7 @@
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="5"/>
@@ -2917,7 +2917,7 @@
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
       <c r="D43" s="5"/>
@@ -2925,7 +2925,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="5"/>
@@ -2933,7 +2933,7 @@
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
       <c r="D45" s="5"/>
@@ -2941,11 +2941,11 @@
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
     </row>
@@ -2966,15 +2966,15 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" style="1"/>
-    <col min="3" max="3" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1"/>
+    <col min="3" max="3" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="54" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>128</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>2021</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>80.803212851405618</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2022</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>82.07630522088354</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2023</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>83.625</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2024</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>83.864541832669318</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>2025</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>86.82113821138212</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="36" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>131</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>132</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>80.803212851405618</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>133</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>72.722891566265062</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>134</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>72.722891566265062</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>135</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>68.682730923694777</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>136</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>84.843373493975903</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>137</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>76.763052208835333</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>138</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>76.763052208835333</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>139</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>80.803212851405618</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>140</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>88.883534136546189</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>141</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>105.0441767068273</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>142</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>80.803212851405618</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>143</v>
       </c>
@@ -3232,15 +3232,15 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" ht="54" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>149</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>1.037037037037037</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>27</v>
       </c>

</xml_diff>